<commit_message>
ingles & sist adm
</commit_message>
<xml_diff>
--- a/1er_cuatrimestre/sist_contable/2_unidad/trabajo_practico/dresch_pedro_tp_asientos_contables.xlsx
+++ b/1er_cuatrimestre/sist_contable/2_unidad/trabajo_practico/dresch_pedro_tp_asientos_contables.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\REPOSITORIOS\repos_facu\3er_anho\1er_cuatrimestre\sist_contable\2_unidad\trabajo_practico\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3E223D9D-8DEE-4A27-B982-09B7EB416FCD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4FC9B979-AC39-4AB2-B692-6BE0C2A28526}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{7772E427-C1A6-4502-A20B-8E0D259B8C62}"/>
   </bookViews>
@@ -288,54 +288,6 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="16" fontId="0" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="16" fontId="0" fillId="3" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="16" fontId="0" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="16" fontId="0" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="16" fontId="0" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="16" fontId="0" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="16" fontId="0" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="16" fontId="0" fillId="3" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="16" fontId="0" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -368,6 +320,54 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="16" fontId="0" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="16" fontId="0" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="16" fontId="0" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="16" fontId="0" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="16" fontId="0" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="16" fontId="0" fillId="3" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="16" fontId="0" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="16" fontId="0" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="16" fontId="0" fillId="3" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -686,7 +686,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{634CB320-D077-4CF4-A785-A3C5E6534657}">
   <dimension ref="A1:P64"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A43" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
       <selection activeCell="M48" sqref="M48"/>
     </sheetView>
   </sheetViews>
@@ -735,10 +735,10 @@
       <c r="M1" s="33"/>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A2" s="25">
+      <c r="A2" s="37">
         <v>44170</v>
       </c>
-      <c r="B2" s="22">
+      <c r="B2" s="34">
         <v>1</v>
       </c>
       <c r="C2" s="2" t="s">
@@ -753,8 +753,8 @@
       </c>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A3" s="26"/>
-      <c r="B3" s="23"/>
+      <c r="A3" s="38"/>
+      <c r="B3" s="35"/>
       <c r="C3" s="2" t="s">
         <v>6</v>
       </c>
@@ -765,23 +765,23 @@
       <c r="F3" s="11">
         <v>2</v>
       </c>
-      <c r="H3" s="47" t="s">
+      <c r="H3" s="31" t="s">
         <v>19</v>
       </c>
-      <c r="I3" s="47" t="s">
+      <c r="I3" s="31" t="s">
         <v>3</v>
       </c>
-      <c r="J3" s="47" t="s">
+      <c r="J3" s="31" t="s">
         <v>4</v>
       </c>
-      <c r="K3" s="47" t="s">
+      <c r="K3" s="31" t="s">
         <v>21</v>
       </c>
-      <c r="L3" s="44"/>
+      <c r="L3" s="28"/>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A4" s="26"/>
-      <c r="B4" s="23"/>
+      <c r="A4" s="38"/>
+      <c r="B4" s="35"/>
       <c r="C4" s="4" t="s">
         <v>16</v>
       </c>
@@ -792,19 +792,19 @@
       <c r="F4" s="11">
         <v>3</v>
       </c>
-      <c r="H4" s="34" t="s">
+      <c r="H4" s="18" t="s">
         <v>5</v>
       </c>
-      <c r="I4" s="35">
+      <c r="I4" s="19">
         <v>30000</v>
       </c>
-      <c r="J4" s="35"/>
-      <c r="K4" s="38"/>
-      <c r="L4" s="44"/>
+      <c r="J4" s="19"/>
+      <c r="K4" s="22"/>
+      <c r="L4" s="28"/>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A5" s="27"/>
-      <c r="B5" s="24"/>
+      <c r="A5" s="39"/>
+      <c r="B5" s="36"/>
       <c r="C5" s="13" t="s">
         <v>7</v>
       </c>
@@ -816,19 +816,19 @@
       <c r="F5" s="11">
         <v>4</v>
       </c>
-      <c r="H5" s="38"/>
-      <c r="I5" s="37">
+      <c r="H5" s="22"/>
+      <c r="I5" s="21">
         <v>3000</v>
       </c>
-      <c r="J5" s="37"/>
-      <c r="K5" s="38"/>
-      <c r="L5" s="44"/>
+      <c r="J5" s="21"/>
+      <c r="K5" s="22"/>
+      <c r="L5" s="28"/>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A6" s="18">
+      <c r="A6" s="40">
         <v>44172</v>
       </c>
-      <c r="B6" s="20">
+      <c r="B6" s="43">
         <v>2</v>
       </c>
       <c r="C6" s="7" t="s">
@@ -842,24 +842,24 @@
       <c r="F6" s="11">
         <v>5</v>
       </c>
-      <c r="H6" s="38"/>
-      <c r="I6" s="45">
+      <c r="H6" s="22"/>
+      <c r="I6" s="29">
         <f>SUM(I4:I5)</f>
         <v>33000</v>
       </c>
-      <c r="J6" s="46">
+      <c r="J6" s="30">
         <f>SUM(J4:J5)</f>
         <v>0</v>
       </c>
-      <c r="K6" s="45">
+      <c r="K6" s="29">
         <f>I6-J6</f>
         <v>33000</v>
       </c>
-      <c r="L6" s="44"/>
+      <c r="L6" s="28"/>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A7" s="32"/>
-      <c r="B7" s="28"/>
+      <c r="A7" s="41"/>
+      <c r="B7" s="44"/>
       <c r="C7" s="14" t="s">
         <v>6</v>
       </c>
@@ -870,15 +870,15 @@
       <c r="F7" s="11">
         <v>2</v>
       </c>
-      <c r="H7" s="44"/>
-      <c r="I7" s="44"/>
-      <c r="J7" s="44"/>
-      <c r="K7" s="44"/>
-      <c r="L7" s="44"/>
+      <c r="H7" s="28"/>
+      <c r="I7" s="28"/>
+      <c r="J7" s="28"/>
+      <c r="K7" s="28"/>
+      <c r="L7" s="28"/>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A8" s="19"/>
-      <c r="B8" s="21"/>
+      <c r="A8" s="42"/>
+      <c r="B8" s="45"/>
       <c r="C8" s="15" t="s">
         <v>16</v>
       </c>
@@ -889,25 +889,25 @@
       <c r="F8" s="11">
         <v>3</v>
       </c>
-      <c r="H8" s="47" t="s">
+      <c r="H8" s="31" t="s">
         <v>19</v>
       </c>
-      <c r="I8" s="47" t="s">
+      <c r="I8" s="31" t="s">
         <v>3</v>
       </c>
-      <c r="J8" s="47" t="s">
+      <c r="J8" s="31" t="s">
         <v>4</v>
       </c>
-      <c r="K8" s="47" t="s">
+      <c r="K8" s="31" t="s">
         <v>21</v>
       </c>
-      <c r="L8" s="44"/>
+      <c r="L8" s="28"/>
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A9" s="25">
+      <c r="A9" s="37">
         <v>44173</v>
       </c>
-      <c r="B9" s="22">
+      <c r="B9" s="34">
         <v>3</v>
       </c>
       <c r="C9" s="4" t="s">
@@ -920,21 +920,21 @@
       <c r="F9" s="11">
         <v>1</v>
       </c>
-      <c r="H9" s="38" t="s">
+      <c r="H9" s="22" t="s">
         <v>6</v>
       </c>
-      <c r="I9" s="35">
+      <c r="I9" s="19">
         <v>15000</v>
       </c>
-      <c r="J9" s="37">
+      <c r="J9" s="21">
         <v>1000</v>
       </c>
-      <c r="K9" s="38"/>
-      <c r="L9" s="44"/>
+      <c r="K9" s="22"/>
+      <c r="L9" s="28"/>
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A10" s="26"/>
-      <c r="B10" s="23"/>
+      <c r="A10" s="38"/>
+      <c r="B10" s="35"/>
       <c r="C10" s="4" t="s">
         <v>9</v>
       </c>
@@ -945,19 +945,19 @@
       <c r="F10" s="11">
         <v>6</v>
       </c>
-      <c r="H10" s="38"/>
-      <c r="I10" s="37">
+      <c r="H10" s="22"/>
+      <c r="I10" s="21">
         <v>1250</v>
       </c>
-      <c r="J10" s="37">
+      <c r="J10" s="21">
         <v>500</v>
       </c>
-      <c r="K10" s="38"/>
-      <c r="L10" s="44"/>
+      <c r="K10" s="22"/>
+      <c r="L10" s="28"/>
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A11" s="26"/>
-      <c r="B11" s="23"/>
+      <c r="A11" s="38"/>
+      <c r="B11" s="35"/>
       <c r="C11" s="16" t="s">
         <v>6</v>
       </c>
@@ -968,19 +968,19 @@
       <c r="F11" s="11">
         <v>2</v>
       </c>
-      <c r="H11" s="38"/>
-      <c r="I11" s="37">
+      <c r="H11" s="22"/>
+      <c r="I11" s="21">
         <v>700</v>
       </c>
-      <c r="J11" s="37">
+      <c r="J11" s="21">
         <v>500</v>
       </c>
-      <c r="K11" s="38"/>
-      <c r="L11" s="44"/>
+      <c r="K11" s="22"/>
+      <c r="L11" s="28"/>
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A12" s="26"/>
-      <c r="B12" s="23"/>
+      <c r="A12" s="38"/>
+      <c r="B12" s="35"/>
       <c r="C12" s="16" t="s">
         <v>16</v>
       </c>
@@ -991,19 +991,19 @@
       <c r="F12" s="11">
         <v>3</v>
       </c>
-      <c r="H12" s="38"/>
-      <c r="I12" s="37">
+      <c r="H12" s="22"/>
+      <c r="I12" s="21">
         <v>2000</v>
       </c>
-      <c r="J12" s="37">
+      <c r="J12" s="21">
         <v>3000</v>
       </c>
-      <c r="K12" s="38"/>
-      <c r="L12" s="44"/>
+      <c r="K12" s="22"/>
+      <c r="L12" s="28"/>
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A13" s="27"/>
-      <c r="B13" s="24"/>
+      <c r="A13" s="39"/>
+      <c r="B13" s="36"/>
       <c r="C13" s="16" t="s">
         <v>10</v>
       </c>
@@ -1014,26 +1014,26 @@
       <c r="F13" s="11">
         <v>7</v>
       </c>
-      <c r="H13" s="38"/>
-      <c r="I13" s="45">
+      <c r="H13" s="22"/>
+      <c r="I13" s="29">
         <f>SUM(I9:I12)</f>
         <v>18950</v>
       </c>
-      <c r="J13" s="45">
+      <c r="J13" s="29">
         <f>SUM(J9:J12)</f>
         <v>5000</v>
       </c>
-      <c r="K13" s="45">
+      <c r="K13" s="29">
         <f>I13-J13</f>
         <v>13950</v>
       </c>
-      <c r="L13" s="44"/>
+      <c r="L13" s="28"/>
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A14" s="18">
+      <c r="A14" s="40">
         <v>44174</v>
       </c>
-      <c r="B14" s="20">
+      <c r="B14" s="43">
         <v>4</v>
       </c>
       <c r="C14" s="9" t="s">
@@ -1047,15 +1047,15 @@
       <c r="F14" s="11">
         <v>2</v>
       </c>
-      <c r="H14" s="44"/>
-      <c r="I14" s="44"/>
-      <c r="J14" s="44"/>
-      <c r="K14" s="44"/>
-      <c r="L14" s="44"/>
+      <c r="H14" s="28"/>
+      <c r="I14" s="28"/>
+      <c r="J14" s="28"/>
+      <c r="K14" s="28"/>
+      <c r="L14" s="28"/>
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A15" s="19"/>
-      <c r="B15" s="21"/>
+      <c r="A15" s="42"/>
+      <c r="B15" s="45"/>
       <c r="C15" s="15" t="s">
         <v>11</v>
       </c>
@@ -1066,25 +1066,25 @@
       <c r="F15" s="11">
         <v>8</v>
       </c>
-      <c r="H15" s="47" t="s">
+      <c r="H15" s="31" t="s">
         <v>19</v>
       </c>
-      <c r="I15" s="47" t="s">
+      <c r="I15" s="31" t="s">
         <v>3</v>
       </c>
-      <c r="J15" s="47" t="s">
+      <c r="J15" s="31" t="s">
         <v>4</v>
       </c>
-      <c r="K15" s="47" t="s">
+      <c r="K15" s="31" t="s">
         <v>21</v>
       </c>
-      <c r="L15" s="44"/>
+      <c r="L15" s="28"/>
     </row>
     <row r="16" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A16" s="25">
+      <c r="A16" s="37">
         <v>44175</v>
       </c>
-      <c r="B16" s="22">
+      <c r="B16" s="34">
         <v>5</v>
       </c>
       <c r="C16" s="4" t="s">
@@ -1098,21 +1098,21 @@
       <c r="F16" s="11">
         <v>5</v>
       </c>
-      <c r="H16" s="39" t="s">
+      <c r="H16" s="23" t="s">
         <v>16</v>
       </c>
-      <c r="I16" s="40">
+      <c r="I16" s="24">
         <v>5000</v>
       </c>
-      <c r="J16" s="37">
+      <c r="J16" s="21">
         <v>1000</v>
       </c>
-      <c r="K16" s="38"/>
-      <c r="L16" s="44"/>
+      <c r="K16" s="22"/>
+      <c r="L16" s="28"/>
     </row>
     <row r="17" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A17" s="27"/>
-      <c r="B17" s="24"/>
+      <c r="A17" s="39"/>
+      <c r="B17" s="36"/>
       <c r="C17" s="16" t="s">
         <v>13</v>
       </c>
@@ -1123,21 +1123,21 @@
       <c r="F17" s="11">
         <v>9</v>
       </c>
-      <c r="H17" s="38"/>
-      <c r="I17" s="37">
+      <c r="H17" s="22"/>
+      <c r="I17" s="21">
         <v>4500</v>
       </c>
-      <c r="J17" s="37">
+      <c r="J17" s="21">
         <v>1500</v>
       </c>
-      <c r="K17" s="38"/>
-      <c r="L17" s="44"/>
+      <c r="K17" s="22"/>
+      <c r="L17" s="28"/>
     </row>
     <row r="18" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A18" s="29">
+      <c r="A18" s="46">
         <v>44180</v>
       </c>
-      <c r="B18" s="20">
+      <c r="B18" s="43">
         <v>6</v>
       </c>
       <c r="C18" s="9" t="s">
@@ -1150,17 +1150,17 @@
       <c r="F18" s="11">
         <v>2</v>
       </c>
-      <c r="H18" s="38"/>
-      <c r="I18" s="38"/>
-      <c r="J18" s="37">
+      <c r="H18" s="22"/>
+      <c r="I18" s="22"/>
+      <c r="J18" s="21">
         <v>4050</v>
       </c>
-      <c r="K18" s="38"/>
-      <c r="L18" s="44"/>
+      <c r="K18" s="22"/>
+      <c r="L18" s="28"/>
     </row>
     <row r="19" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A19" s="30"/>
-      <c r="B19" s="28"/>
+      <c r="A19" s="47"/>
+      <c r="B19" s="44"/>
       <c r="C19" s="9" t="s">
         <v>14</v>
       </c>
@@ -1171,24 +1171,24 @@
       <c r="F19" s="11">
         <v>10</v>
       </c>
-      <c r="H19" s="38"/>
-      <c r="I19" s="45">
+      <c r="H19" s="22"/>
+      <c r="I19" s="29">
         <f>SUM(I16:I18)</f>
         <v>9500</v>
       </c>
-      <c r="J19" s="45">
+      <c r="J19" s="29">
         <f>SUM(J16:J18)</f>
         <v>6550</v>
       </c>
-      <c r="K19" s="45">
+      <c r="K19" s="29">
         <f>I19-J19</f>
         <v>2950</v>
       </c>
-      <c r="L19" s="44"/>
+      <c r="L19" s="28"/>
     </row>
     <row r="20" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A20" s="30"/>
-      <c r="B20" s="28"/>
+      <c r="A20" s="47"/>
+      <c r="B20" s="44"/>
       <c r="C20" s="9" t="s">
         <v>15</v>
       </c>
@@ -1199,15 +1199,15 @@
       <c r="F20" s="11">
         <v>11</v>
       </c>
-      <c r="H20" s="44"/>
-      <c r="I20" s="44"/>
-      <c r="J20" s="44"/>
-      <c r="K20" s="44"/>
-      <c r="L20" s="44"/>
+      <c r="H20" s="28"/>
+      <c r="I20" s="28"/>
+      <c r="J20" s="28"/>
+      <c r="K20" s="28"/>
+      <c r="L20" s="28"/>
     </row>
     <row r="21" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A21" s="31"/>
-      <c r="B21" s="21"/>
+      <c r="A21" s="48"/>
+      <c r="B21" s="45"/>
       <c r="C21" s="15" t="s">
         <v>11</v>
       </c>
@@ -1219,25 +1219,25 @@
       <c r="F21" s="11">
         <v>8</v>
       </c>
-      <c r="H21" s="47" t="s">
+      <c r="H21" s="31" t="s">
         <v>19</v>
       </c>
-      <c r="I21" s="47" t="s">
+      <c r="I21" s="31" t="s">
         <v>3</v>
       </c>
-      <c r="J21" s="47" t="s">
+      <c r="J21" s="31" t="s">
         <v>4</v>
       </c>
-      <c r="K21" s="47" t="s">
+      <c r="K21" s="31" t="s">
         <v>21</v>
       </c>
-      <c r="L21" s="44"/>
+      <c r="L21" s="28"/>
     </row>
     <row r="22" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A22" s="25">
+      <c r="A22" s="37">
         <v>44185</v>
       </c>
-      <c r="B22" s="22">
+      <c r="B22" s="34">
         <v>7</v>
       </c>
       <c r="C22" s="2" t="s">
@@ -1251,19 +1251,19 @@
       <c r="F22" s="11">
         <v>3</v>
       </c>
-      <c r="H22" s="41" t="s">
+      <c r="H22" s="25" t="s">
         <v>7</v>
       </c>
-      <c r="I22" s="37"/>
-      <c r="J22" s="37">
+      <c r="I22" s="21"/>
+      <c r="J22" s="21">
         <v>50000</v>
       </c>
-      <c r="K22" s="38"/>
-      <c r="L22" s="44"/>
+      <c r="K22" s="22"/>
+      <c r="L22" s="28"/>
     </row>
     <row r="23" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A23" s="26"/>
-      <c r="B23" s="23"/>
+      <c r="A23" s="38"/>
+      <c r="B23" s="35"/>
       <c r="C23" s="13" t="s">
         <v>14</v>
       </c>
@@ -1274,24 +1274,24 @@
       <c r="F23" s="11">
         <v>10</v>
       </c>
-      <c r="H23" s="38"/>
-      <c r="I23" s="45">
+      <c r="H23" s="22"/>
+      <c r="I23" s="29">
         <f>SUM(I22)</f>
         <v>0</v>
       </c>
-      <c r="J23" s="45">
+      <c r="J23" s="29">
         <f>SUM(J22)</f>
         <v>50000</v>
       </c>
-      <c r="K23" s="45">
+      <c r="K23" s="29">
         <f>I23-J23</f>
         <v>-50000</v>
       </c>
-      <c r="L23" s="44"/>
+      <c r="L23" s="28"/>
     </row>
     <row r="24" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A24" s="27"/>
-      <c r="B24" s="24"/>
+      <c r="A24" s="39"/>
+      <c r="B24" s="36"/>
       <c r="C24" s="13" t="s">
         <v>6</v>
       </c>
@@ -1302,17 +1302,17 @@
       <c r="F24" s="11">
         <v>2</v>
       </c>
-      <c r="H24" s="44"/>
-      <c r="I24" s="44"/>
-      <c r="J24" s="44"/>
-      <c r="K24" s="44"/>
-      <c r="L24" s="44"/>
+      <c r="H24" s="28"/>
+      <c r="I24" s="28"/>
+      <c r="J24" s="28"/>
+      <c r="K24" s="28"/>
+      <c r="L24" s="28"/>
     </row>
     <row r="25" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A25" s="18">
+      <c r="A25" s="40">
         <v>44185</v>
       </c>
-      <c r="B25" s="20">
+      <c r="B25" s="43">
         <v>8</v>
       </c>
       <c r="C25" s="7" t="s">
@@ -1326,23 +1326,23 @@
       <c r="F25" s="11">
         <v>12</v>
       </c>
-      <c r="H25" s="47" t="s">
+      <c r="H25" s="31" t="s">
         <v>19</v>
       </c>
-      <c r="I25" s="47" t="s">
+      <c r="I25" s="31" t="s">
         <v>3</v>
       </c>
-      <c r="J25" s="47" t="s">
+      <c r="J25" s="31" t="s">
         <v>4</v>
       </c>
-      <c r="K25" s="47" t="s">
+      <c r="K25" s="31" t="s">
         <v>21</v>
       </c>
-      <c r="L25" s="44"/>
+      <c r="L25" s="28"/>
     </row>
     <row r="26" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A26" s="19"/>
-      <c r="B26" s="21"/>
+      <c r="A26" s="42"/>
+      <c r="B26" s="45"/>
       <c r="C26" s="14" t="s">
         <v>11</v>
       </c>
@@ -1354,22 +1354,22 @@
       <c r="F26" s="11">
         <v>8</v>
       </c>
-      <c r="H26" s="34" t="s">
+      <c r="H26" s="18" t="s">
         <v>8</v>
       </c>
-      <c r="I26" s="37">
+      <c r="I26" s="21">
         <f>100*20</f>
         <v>2000</v>
       </c>
-      <c r="J26" s="37"/>
-      <c r="K26" s="38"/>
-      <c r="L26" s="44"/>
+      <c r="J26" s="21"/>
+      <c r="K26" s="22"/>
+      <c r="L26" s="28"/>
     </row>
     <row r="27" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A27" s="25">
+      <c r="A27" s="37">
         <v>44186</v>
       </c>
-      <c r="B27" s="22">
+      <c r="B27" s="34">
         <v>9</v>
       </c>
       <c r="C27" s="2" t="s">
@@ -1382,18 +1382,18 @@
       <c r="F27" s="11">
         <v>7</v>
       </c>
-      <c r="H27" s="38"/>
-      <c r="I27" s="37">
+      <c r="H27" s="22"/>
+      <c r="I27" s="21">
         <f>300*20</f>
         <v>6000</v>
       </c>
-      <c r="J27" s="37"/>
-      <c r="K27" s="38"/>
-      <c r="L27" s="44"/>
+      <c r="J27" s="21"/>
+      <c r="K27" s="22"/>
+      <c r="L27" s="28"/>
     </row>
     <row r="28" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A28" s="27"/>
-      <c r="B28" s="24"/>
+      <c r="A28" s="39"/>
+      <c r="B28" s="36"/>
       <c r="C28" s="13" t="s">
         <v>16</v>
       </c>
@@ -1404,26 +1404,26 @@
       <c r="F28" s="11">
         <v>3</v>
       </c>
-      <c r="H28" s="38"/>
-      <c r="I28" s="45">
+      <c r="H28" s="22"/>
+      <c r="I28" s="29">
         <f>SUM(I26:I27)</f>
         <v>8000</v>
       </c>
-      <c r="J28" s="45">
+      <c r="J28" s="29">
         <f>SUM(J26:J27)</f>
         <v>0</v>
       </c>
-      <c r="K28" s="45">
+      <c r="K28" s="29">
         <f>I28-J28</f>
         <v>8000</v>
       </c>
-      <c r="L28" s="44"/>
+      <c r="L28" s="28"/>
     </row>
     <row r="29" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A29" s="18">
+      <c r="A29" s="40">
         <v>44187</v>
       </c>
-      <c r="B29" s="20">
+      <c r="B29" s="43">
         <v>10</v>
       </c>
       <c r="C29" s="7" t="s">
@@ -1436,19 +1436,19 @@
       <c r="F29" s="11">
         <v>9</v>
       </c>
-      <c r="H29" s="44"/>
-      <c r="I29" s="44"/>
-      <c r="J29" s="44"/>
-      <c r="K29" s="44"/>
-      <c r="L29" s="44"/>
-      <c r="M29" s="44"/>
-      <c r="N29" s="44"/>
-      <c r="O29" s="44"/>
-      <c r="P29" s="44"/>
+      <c r="H29" s="28"/>
+      <c r="I29" s="28"/>
+      <c r="J29" s="28"/>
+      <c r="K29" s="28"/>
+      <c r="L29" s="28"/>
+      <c r="M29" s="28"/>
+      <c r="N29" s="28"/>
+      <c r="O29" s="28"/>
+      <c r="P29" s="28"/>
     </row>
     <row r="30" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A30" s="19"/>
-      <c r="B30" s="21"/>
+      <c r="A30" s="42"/>
+      <c r="B30" s="45"/>
       <c r="C30" s="14" t="s">
         <v>6</v>
       </c>
@@ -1459,29 +1459,29 @@
       <c r="F30" s="11">
         <v>2</v>
       </c>
-      <c r="H30" s="48" t="s">
+      <c r="H30" s="32" t="s">
         <v>19</v>
       </c>
-      <c r="I30" s="48" t="s">
+      <c r="I30" s="32" t="s">
         <v>3</v>
       </c>
-      <c r="J30" s="48" t="s">
+      <c r="J30" s="32" t="s">
         <v>4</v>
       </c>
-      <c r="K30" s="48" t="s">
+      <c r="K30" s="32" t="s">
         <v>21</v>
       </c>
-      <c r="L30" s="44"/>
-      <c r="M30" s="44"/>
-      <c r="N30" s="44"/>
-      <c r="O30" s="44"/>
-      <c r="P30" s="44"/>
+      <c r="L30" s="28"/>
+      <c r="M30" s="28"/>
+      <c r="N30" s="28"/>
+      <c r="O30" s="28"/>
+      <c r="P30" s="28"/>
     </row>
     <row r="31" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A31" s="25">
+      <c r="A31" s="37">
         <v>44188</v>
       </c>
-      <c r="B31" s="22">
+      <c r="B31" s="34">
         <v>11</v>
       </c>
       <c r="C31" s="2" t="s">
@@ -1494,23 +1494,23 @@
       <c r="F31" s="11">
         <v>2</v>
       </c>
-      <c r="H31" s="39" t="s">
+      <c r="H31" s="23" t="s">
         <v>9</v>
       </c>
-      <c r="I31" s="37">
+      <c r="I31" s="21">
         <v>40</v>
       </c>
-      <c r="J31" s="37"/>
-      <c r="K31" s="38"/>
-      <c r="L31" s="44"/>
-      <c r="M31" s="44"/>
-      <c r="N31" s="44"/>
-      <c r="O31" s="44"/>
-      <c r="P31" s="44"/>
+      <c r="J31" s="21"/>
+      <c r="K31" s="22"/>
+      <c r="L31" s="28"/>
+      <c r="M31" s="28"/>
+      <c r="N31" s="28"/>
+      <c r="O31" s="28"/>
+      <c r="P31" s="28"/>
     </row>
     <row r="32" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A32" s="26"/>
-      <c r="B32" s="23"/>
+      <c r="A32" s="38"/>
+      <c r="B32" s="35"/>
       <c r="C32" s="12" t="s">
         <v>14</v>
       </c>
@@ -1521,28 +1521,28 @@
       <c r="F32" s="11">
         <v>10</v>
       </c>
-      <c r="H32" s="38"/>
-      <c r="I32" s="45">
+      <c r="H32" s="22"/>
+      <c r="I32" s="29">
         <f>SUM(I31)</f>
         <v>40</v>
       </c>
-      <c r="J32" s="45">
+      <c r="J32" s="29">
         <f>SUM(J31)</f>
         <v>0</v>
       </c>
-      <c r="K32" s="45">
+      <c r="K32" s="29">
         <f>I32-J32</f>
         <v>40</v>
       </c>
-      <c r="L32" s="44"/>
-      <c r="M32" s="44"/>
-      <c r="N32" s="44"/>
-      <c r="O32" s="44"/>
-      <c r="P32" s="44"/>
+      <c r="L32" s="28"/>
+      <c r="M32" s="28"/>
+      <c r="N32" s="28"/>
+      <c r="O32" s="28"/>
+      <c r="P32" s="28"/>
     </row>
     <row r="33" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A33" s="27"/>
-      <c r="B33" s="24"/>
+      <c r="A33" s="39"/>
+      <c r="B33" s="36"/>
       <c r="C33" s="13" t="s">
         <v>18</v>
       </c>
@@ -1553,72 +1553,72 @@
       <c r="F33" s="11">
         <v>13</v>
       </c>
-      <c r="H33" s="44"/>
-      <c r="I33" s="44"/>
-      <c r="J33" s="44"/>
-      <c r="K33" s="44"/>
-      <c r="L33" s="44"/>
-      <c r="M33" s="44"/>
-      <c r="N33" s="44"/>
-      <c r="O33" s="44"/>
-      <c r="P33" s="44"/>
+      <c r="H33" s="28"/>
+      <c r="I33" s="28"/>
+      <c r="J33" s="28"/>
+      <c r="K33" s="28"/>
+      <c r="L33" s="28"/>
+      <c r="M33" s="28"/>
+      <c r="N33" s="28"/>
+      <c r="O33" s="28"/>
+      <c r="P33" s="28"/>
     </row>
     <row r="34" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="L34" s="44"/>
-      <c r="M34" s="44"/>
-      <c r="N34" s="44"/>
-      <c r="O34" s="44"/>
-      <c r="P34" s="44"/>
+      <c r="L34" s="28"/>
+      <c r="M34" s="28"/>
+      <c r="N34" s="28"/>
+      <c r="O34" s="28"/>
+      <c r="P34" s="28"/>
     </row>
     <row r="35" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="H35" s="48" t="s">
+      <c r="H35" s="32" t="s">
         <v>19</v>
       </c>
-      <c r="I35" s="48" t="s">
+      <c r="I35" s="32" t="s">
         <v>3</v>
       </c>
-      <c r="J35" s="48" t="s">
+      <c r="J35" s="32" t="s">
         <v>4</v>
       </c>
-      <c r="K35" s="48" t="s">
+      <c r="K35" s="32" t="s">
         <v>21</v>
       </c>
-      <c r="L35" s="44"/>
-      <c r="M35" s="44"/>
-      <c r="N35" s="44"/>
-      <c r="O35" s="44"/>
-      <c r="P35" s="44"/>
+      <c r="L35" s="28"/>
+      <c r="M35" s="28"/>
+      <c r="N35" s="28"/>
+      <c r="O35" s="28"/>
+      <c r="P35" s="28"/>
     </row>
     <row r="36" spans="1:16" ht="16.5" x14ac:dyDescent="0.25">
       <c r="G36" s="10"/>
-      <c r="H36" s="43" t="s">
+      <c r="H36" s="27" t="s">
         <v>10</v>
       </c>
-      <c r="I36" s="37">
+      <c r="I36" s="21">
         <v>4050</v>
       </c>
-      <c r="J36" s="37">
+      <c r="J36" s="21">
         <v>1040</v>
       </c>
-      <c r="K36" s="38"/>
-      <c r="L36" s="44"/>
-      <c r="M36" s="44"/>
-      <c r="N36" s="44"/>
-      <c r="O36" s="44"/>
-      <c r="P36" s="44"/>
+      <c r="K36" s="22"/>
+      <c r="L36" s="28"/>
+      <c r="M36" s="28"/>
+      <c r="N36" s="28"/>
+      <c r="O36" s="28"/>
+      <c r="P36" s="28"/>
     </row>
     <row r="37" spans="1:16" ht="16.5" x14ac:dyDescent="0.25">
       <c r="G37" s="10"/>
-      <c r="H37" s="38"/>
-      <c r="I37" s="45">
+      <c r="H37" s="22"/>
+      <c r="I37" s="29">
         <f>SUM(I36)</f>
         <v>4050</v>
       </c>
-      <c r="J37" s="45">
+      <c r="J37" s="29">
         <f>SUM(J36)</f>
         <v>1040</v>
       </c>
-      <c r="K37" s="45">
+      <c r="K37" s="29">
         <f>I37-J37</f>
         <v>3010</v>
       </c>
@@ -1628,318 +1628,319 @@
     </row>
     <row r="39" spans="1:16" ht="16.5" x14ac:dyDescent="0.25">
       <c r="G39" s="10"/>
-      <c r="H39" s="48" t="s">
+      <c r="H39" s="32" t="s">
         <v>19</v>
       </c>
-      <c r="I39" s="48" t="s">
+      <c r="I39" s="32" t="s">
         <v>3</v>
       </c>
-      <c r="J39" s="48" t="s">
+      <c r="J39" s="32" t="s">
         <v>4</v>
       </c>
-      <c r="K39" s="48" t="s">
+      <c r="K39" s="32" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="40" spans="1:16" ht="16.5" x14ac:dyDescent="0.25">
       <c r="G40" s="10"/>
-      <c r="H40" s="36" t="s">
+      <c r="H40" s="20" t="s">
         <v>11</v>
       </c>
-      <c r="I40" s="37"/>
-      <c r="J40" s="37">
+      <c r="I40" s="21"/>
+      <c r="J40" s="21">
         <v>1250</v>
       </c>
-      <c r="K40" s="38"/>
+      <c r="K40" s="22"/>
     </row>
     <row r="41" spans="1:16" ht="16.5" x14ac:dyDescent="0.25">
       <c r="G41" s="10"/>
-      <c r="H41" s="38"/>
-      <c r="I41" s="37"/>
-      <c r="J41" s="37">
+      <c r="H41" s="22"/>
+      <c r="I41" s="21"/>
+      <c r="J41" s="21">
         <f>200*25</f>
         <v>5000</v>
       </c>
-      <c r="K41" s="38"/>
+      <c r="K41" s="22"/>
     </row>
     <row r="42" spans="1:16" ht="16.5" x14ac:dyDescent="0.25">
       <c r="G42" s="10"/>
-      <c r="H42" s="38"/>
-      <c r="I42" s="37"/>
-      <c r="J42" s="37">
+      <c r="H42" s="22"/>
+      <c r="I42" s="21"/>
+      <c r="J42" s="21">
         <f>20*25</f>
         <v>500</v>
       </c>
-      <c r="K42" s="38"/>
+      <c r="K42" s="22"/>
     </row>
     <row r="43" spans="1:16" ht="16.5" x14ac:dyDescent="0.25">
       <c r="G43" s="10"/>
-      <c r="H43" s="38"/>
-      <c r="I43" s="45">
+      <c r="H43" s="22"/>
+      <c r="I43" s="29">
         <f>SUM(I40:I42)</f>
         <v>0</v>
       </c>
-      <c r="J43" s="45">
+      <c r="J43" s="29">
         <f>SUM(J40:J42)</f>
         <v>6750</v>
       </c>
-      <c r="K43" s="45">
+      <c r="K43" s="29">
         <f>I43-J43</f>
         <v>-6750</v>
       </c>
     </row>
     <row r="44" spans="1:16" ht="16.5" x14ac:dyDescent="0.25">
       <c r="G44" s="10"/>
-      <c r="H44" s="44"/>
-      <c r="I44" s="44"/>
-      <c r="J44" s="44"/>
-      <c r="K44" s="44"/>
+      <c r="H44" s="28"/>
+      <c r="I44" s="28"/>
+      <c r="J44" s="28"/>
+      <c r="K44" s="28"/>
     </row>
     <row r="45" spans="1:16" ht="16.5" x14ac:dyDescent="0.25">
       <c r="G45" s="10"/>
-      <c r="H45" s="48" t="s">
+      <c r="H45" s="32" t="s">
         <v>19</v>
       </c>
-      <c r="I45" s="48" t="s">
+      <c r="I45" s="32" t="s">
         <v>3</v>
       </c>
-      <c r="J45" s="48" t="s">
+      <c r="J45" s="32" t="s">
         <v>4</v>
       </c>
-      <c r="K45" s="48" t="s">
+      <c r="K45" s="32" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="46" spans="1:16" ht="16.5" x14ac:dyDescent="0.25">
       <c r="G46" s="10"/>
-      <c r="H46" s="36" t="s">
+      <c r="H46" s="20" t="s">
         <v>13</v>
       </c>
-      <c r="I46" s="37">
+      <c r="I46" s="21">
         <v>3000</v>
       </c>
-      <c r="J46" s="37">
+      <c r="J46" s="21">
         <v>6000</v>
       </c>
-      <c r="K46" s="38"/>
+      <c r="K46" s="22"/>
     </row>
     <row r="47" spans="1:16" ht="16.5" x14ac:dyDescent="0.25">
       <c r="G47" s="10"/>
-      <c r="H47" s="38"/>
-      <c r="I47" s="45">
+      <c r="H47" s="22"/>
+      <c r="I47" s="29">
         <f>SUM(I46)</f>
         <v>3000</v>
       </c>
-      <c r="J47" s="45">
+      <c r="J47" s="29">
         <f>SUM(J46)</f>
         <v>6000</v>
       </c>
-      <c r="K47" s="45">
+      <c r="K47" s="29">
         <f>I47-J47</f>
         <v>-3000</v>
       </c>
     </row>
     <row r="48" spans="1:16" ht="16.5" x14ac:dyDescent="0.25">
       <c r="G48" s="10"/>
-      <c r="H48" s="44"/>
-      <c r="I48" s="44"/>
-      <c r="J48" s="44"/>
-      <c r="K48" s="44"/>
+      <c r="H48" s="28"/>
+      <c r="I48" s="28"/>
+      <c r="J48" s="28"/>
+      <c r="K48" s="28"/>
     </row>
     <row r="49" spans="7:11" ht="16.5" x14ac:dyDescent="0.25">
       <c r="G49" s="10"/>
-      <c r="H49" s="48" t="s">
+      <c r="H49" s="32" t="s">
         <v>19</v>
       </c>
-      <c r="I49" s="48" t="s">
+      <c r="I49" s="32" t="s">
         <v>3</v>
       </c>
-      <c r="J49" s="48" t="s">
+      <c r="J49" s="32" t="s">
         <v>4</v>
       </c>
-      <c r="K49" s="48" t="s">
+      <c r="K49" s="32" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="50" spans="7:11" ht="16.5" x14ac:dyDescent="0.25">
       <c r="G50" s="10"/>
-      <c r="H50" s="39" t="s">
+      <c r="H50" s="23" t="s">
         <v>14</v>
       </c>
-      <c r="I50" s="37">
+      <c r="I50" s="21">
         <v>4000</v>
       </c>
-      <c r="J50" s="37">
+      <c r="J50" s="21">
         <v>4000</v>
       </c>
-      <c r="K50" s="38"/>
+      <c r="K50" s="22"/>
     </row>
     <row r="51" spans="7:11" ht="16.5" x14ac:dyDescent="0.25">
       <c r="G51" s="10"/>
-      <c r="H51" s="38"/>
-      <c r="I51" s="37">
+      <c r="H51" s="22"/>
+      <c r="I51" s="21">
         <v>2000</v>
       </c>
-      <c r="J51" s="38"/>
-      <c r="K51" s="38"/>
+      <c r="J51" s="22"/>
+      <c r="K51" s="22"/>
     </row>
     <row r="52" spans="7:11" ht="16.5" x14ac:dyDescent="0.25">
       <c r="G52" s="10"/>
-      <c r="H52" s="38"/>
-      <c r="I52" s="45">
+      <c r="H52" s="22"/>
+      <c r="I52" s="29">
         <f>SUM(I50:I51)</f>
         <v>6000</v>
       </c>
-      <c r="J52" s="45">
+      <c r="J52" s="29">
         <f>SUM(J50:J51)</f>
         <v>4000</v>
       </c>
-      <c r="K52" s="45">
+      <c r="K52" s="29">
         <f>I52-J52</f>
         <v>2000</v>
       </c>
     </row>
     <row r="53" spans="7:11" ht="16.5" x14ac:dyDescent="0.25">
       <c r="G53" s="10"/>
-      <c r="H53" s="44"/>
-      <c r="I53" s="44"/>
-      <c r="J53" s="44"/>
-      <c r="K53" s="44"/>
+      <c r="H53" s="28"/>
+      <c r="I53" s="28"/>
+      <c r="J53" s="28"/>
+      <c r="K53" s="28"/>
     </row>
     <row r="54" spans="7:11" ht="16.5" x14ac:dyDescent="0.25">
       <c r="G54" s="10"/>
-      <c r="H54" s="48" t="s">
+      <c r="H54" s="32" t="s">
         <v>19</v>
       </c>
-      <c r="I54" s="48" t="s">
+      <c r="I54" s="32" t="s">
         <v>3</v>
       </c>
-      <c r="J54" s="48" t="s">
+      <c r="J54" s="32" t="s">
         <v>4</v>
       </c>
-      <c r="K54" s="48" t="s">
+      <c r="K54" s="32" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="55" spans="7:11" ht="16.5" x14ac:dyDescent="0.25">
       <c r="G55" s="10"/>
-      <c r="H55" s="39" t="s">
+      <c r="H55" s="23" t="s">
         <v>15</v>
       </c>
-      <c r="I55" s="37">
+      <c r="I55" s="21">
         <v>300</v>
       </c>
-      <c r="J55" s="37"/>
-      <c r="K55" s="37"/>
+      <c r="J55" s="21"/>
+      <c r="K55" s="21"/>
     </row>
     <row r="56" spans="7:11" ht="16.5" x14ac:dyDescent="0.25">
       <c r="G56" s="10"/>
-      <c r="H56" s="38"/>
-      <c r="I56" s="46">
+      <c r="H56" s="22"/>
+      <c r="I56" s="30">
         <v>300</v>
       </c>
-      <c r="J56" s="46"/>
-      <c r="K56" s="46">
+      <c r="J56" s="30"/>
+      <c r="K56" s="30">
         <v>300</v>
       </c>
     </row>
     <row r="57" spans="7:11" ht="16.5" x14ac:dyDescent="0.25">
       <c r="G57" s="10"/>
-      <c r="H57" s="44"/>
-      <c r="I57" s="44"/>
-      <c r="J57" s="44"/>
-      <c r="K57" s="44"/>
+      <c r="H57" s="28"/>
+      <c r="I57" s="28"/>
+      <c r="J57" s="28"/>
+      <c r="K57" s="28"/>
     </row>
     <row r="58" spans="7:11" ht="16.5" x14ac:dyDescent="0.25">
       <c r="G58" s="10"/>
-      <c r="H58" s="48" t="s">
+      <c r="H58" s="32" t="s">
         <v>19</v>
       </c>
-      <c r="I58" s="48" t="s">
+      <c r="I58" s="32" t="s">
         <v>3</v>
       </c>
-      <c r="J58" s="48" t="s">
+      <c r="J58" s="32" t="s">
         <v>4</v>
       </c>
-      <c r="K58" s="48" t="s">
+      <c r="K58" s="32" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="59" spans="7:11" ht="16.5" x14ac:dyDescent="0.25">
       <c r="G59" s="10"/>
-      <c r="H59" s="34" t="s">
+      <c r="H59" s="18" t="s">
         <v>17</v>
       </c>
-      <c r="I59" s="37">
+      <c r="I59" s="21">
         <f>20*25</f>
         <v>500</v>
       </c>
-      <c r="J59" s="37"/>
-      <c r="K59" s="37"/>
+      <c r="J59" s="21"/>
+      <c r="K59" s="21"/>
     </row>
     <row r="60" spans="7:11" ht="16.5" x14ac:dyDescent="0.25">
       <c r="G60" s="10"/>
-      <c r="H60" s="38"/>
-      <c r="I60" s="46">
+      <c r="H60" s="22"/>
+      <c r="I60" s="30">
         <v>500</v>
       </c>
-      <c r="J60" s="46"/>
-      <c r="K60" s="46">
+      <c r="J60" s="30"/>
+      <c r="K60" s="30">
         <v>500</v>
       </c>
     </row>
     <row r="61" spans="7:11" ht="16.5" x14ac:dyDescent="0.25">
       <c r="G61" s="10"/>
-      <c r="H61" s="44"/>
-      <c r="I61" s="44"/>
-      <c r="J61" s="44"/>
-      <c r="K61" s="44"/>
+      <c r="H61" s="28"/>
+      <c r="I61" s="28"/>
+      <c r="J61" s="28"/>
+      <c r="K61" s="28"/>
     </row>
     <row r="62" spans="7:11" ht="16.5" x14ac:dyDescent="0.25">
       <c r="G62" s="10"/>
-      <c r="H62" s="48" t="s">
+      <c r="H62" s="32" t="s">
         <v>19</v>
       </c>
-      <c r="I62" s="48" t="s">
+      <c r="I62" s="32" t="s">
         <v>3</v>
       </c>
-      <c r="J62" s="48" t="s">
+      <c r="J62" s="32" t="s">
         <v>4</v>
       </c>
-      <c r="K62" s="48" t="s">
+      <c r="K62" s="32" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="63" spans="7:11" ht="16.5" x14ac:dyDescent="0.25">
       <c r="G63" s="10"/>
-      <c r="H63" s="42" t="s">
+      <c r="H63" s="26" t="s">
         <v>18</v>
       </c>
-      <c r="I63" s="37"/>
-      <c r="J63" s="37">
+      <c r="I63" s="21"/>
+      <c r="J63" s="21">
         <v>4000</v>
       </c>
-      <c r="K63" s="37"/>
+      <c r="K63" s="21"/>
     </row>
     <row r="64" spans="7:11" ht="16.5" x14ac:dyDescent="0.25">
       <c r="G64" s="10"/>
-      <c r="H64" s="38"/>
-      <c r="I64" s="46"/>
-      <c r="J64" s="46">
+      <c r="H64" s="22"/>
+      <c r="I64" s="30"/>
+      <c r="J64" s="30">
         <v>4000</v>
       </c>
-      <c r="K64" s="46">
+      <c r="K64" s="30">
         <f>I64-J64</f>
         <v>-4000</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="23">
-    <mergeCell ref="H1:M1"/>
-    <mergeCell ref="B2:B5"/>
-    <mergeCell ref="A2:A5"/>
-    <mergeCell ref="A6:A8"/>
-    <mergeCell ref="B6:B8"/>
+    <mergeCell ref="A29:A30"/>
+    <mergeCell ref="B29:B30"/>
+    <mergeCell ref="B31:B33"/>
+    <mergeCell ref="A31:A33"/>
+    <mergeCell ref="A27:A28"/>
+    <mergeCell ref="B27:B28"/>
     <mergeCell ref="A9:A13"/>
     <mergeCell ref="B9:B13"/>
     <mergeCell ref="B22:B24"/>
@@ -1952,12 +1953,11 @@
     <mergeCell ref="B16:B17"/>
     <mergeCell ref="B18:B21"/>
     <mergeCell ref="A18:A21"/>
-    <mergeCell ref="A29:A30"/>
-    <mergeCell ref="B29:B30"/>
-    <mergeCell ref="B31:B33"/>
-    <mergeCell ref="A31:A33"/>
-    <mergeCell ref="A27:A28"/>
-    <mergeCell ref="B27:B28"/>
+    <mergeCell ref="H1:M1"/>
+    <mergeCell ref="B2:B5"/>
+    <mergeCell ref="A2:A5"/>
+    <mergeCell ref="A6:A8"/>
+    <mergeCell ref="B6:B8"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="landscape" r:id="rId1"/>

</xml_diff>